<commit_message>
another excel update again
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE724CF-6D87-4574-A796-0E0BC1F79C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD5D5FA-872A-406F-A2C0-C2267C554AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -321,9 +321,6 @@
     <t>""</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -346,9 +343,6 @@
   </si>
   <si>
     <t>expected result</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>"M"</t>
@@ -570,9 +564,6 @@
     <t>16. inStock = -1</t>
   </si>
   <si>
-    <t>17. inStock = 1</t>
-  </si>
-  <si>
     <t>18. inStock = 100</t>
   </si>
   <si>
@@ -670,9 +661,6 @@
   </si>
   <si>
     <t>1,7, 14,20,25,40</t>
-  </si>
-  <si>
-    <t>2,9,15,21,35,39</t>
   </si>
   <si>
     <t>3,10,18,23,31,41</t>
@@ -802,12 +790,45 @@
       <t>, 11,14</t>
     </r>
   </si>
+  <si>
+    <t>"festar"</t>
+  </si>
+  <si>
+    <t>17. inStock = 1, min = 2, max = 3</t>
+  </si>
+  <si>
+    <r>
+      <t>2,9,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,21,35,39</t>
+    </r>
+  </si>
+  <si>
+    <t>In stock must be between min and max!</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1001,6 +1022,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1543,7 +1571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1568,9 +1596,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1631,9 +1656,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1688,6 +1710,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1703,6 +1734,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1727,35 +1803,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1769,25 +1824,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1799,8 +1839,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1817,38 +1875,80 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1865,7 +1965,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1875,95 +1974,25 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2288,24 +2317,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="67"/>
-      <c r="H1" s="38" t="s">
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="68"/>
+      <c r="H1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H2" s="68" t="s">
+      <c r="H2" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H3" s="2"/>
@@ -2321,7 +2350,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J4" s="2">
         <v>233</v>
@@ -2332,19 +2361,19 @@
         <v>6</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J5" s="2">
         <v>233</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="24"/>
+      <c r="B6" s="23"/>
       <c r="H6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J6" s="2">
         <v>233</v>
@@ -2352,7 +2381,7 @@
     </row>
     <row r="7" spans="2:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="35" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2401,7 +2430,7 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2413,7 +2442,7 @@
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="35" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2423,7 +2452,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="33" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2467,25 +2496,25 @@
       <c r="O23" s="1"/>
     </row>
     <row r="24" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="64" t="s">
+      <c r="A24" s="34"/>
+      <c r="B24" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="64"/>
-      <c r="N24" s="64"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="65"/>
+      <c r="L24" s="65"/>
+      <c r="M24" s="65"/>
+      <c r="N24" s="65"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C26" s="37"/>
+      <c r="C26" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2506,7 +2535,7 @@
   <dimension ref="B1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10:Q10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2528,131 +2557,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
     </row>
     <row r="3" spans="2:17" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="88"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="89" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="G5" s="90" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="90"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="90"/>
+      <c r="Q5" s="90"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="96" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="99"/>
+      <c r="N6" s="99"/>
+      <c r="O6" s="76"/>
+      <c r="P6" s="98" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="98"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="41">
+        <v>1</v>
+      </c>
+      <c r="C7" s="85" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="97"/>
+      <c r="I7" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="72"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="G5" s="74" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="74"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="75" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="87" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="85" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="86"/>
-      <c r="P6" s="89" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q6" s="89"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="43">
-        <v>1</v>
-      </c>
-      <c r="C7" s="69" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="13" t="s">
+      <c r="L7" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="M7" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="K7" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="L7" s="13" t="s">
+      <c r="N7" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="M7" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="N7" s="85" t="s">
-        <v>90</v>
-      </c>
-      <c r="O7" s="86"/>
-      <c r="P7" s="85" t="s">
+      <c r="O7" s="76"/>
+      <c r="P7" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="Q7" s="86"/>
+      <c r="Q7" s="76"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="44">
+      <c r="B8" s="42">
         <v>2</v>
       </c>
-      <c r="C8" s="69"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G8" s="13">
+        <v>93</v>
+      </c>
+      <c r="G8" s="12">
         <v>1</v>
       </c>
-      <c r="H8" s="45" t="s">
-        <v>85</v>
+      <c r="H8" s="43" t="s">
+        <v>83</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J8" s="2">
         <v>100</v>
@@ -2666,33 +2695,33 @@
       <c r="M8" s="2">
         <v>30</v>
       </c>
-      <c r="N8" s="83">
+      <c r="N8" s="93">
         <v>5</v>
       </c>
-      <c r="O8" s="84" t="s">
+      <c r="O8" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="83" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q8" s="84"/>
+      <c r="P8" s="93" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q8" s="94"/>
     </row>
     <row r="9" spans="2:17" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="43">
+      <c r="B9" s="41">
         <v>3</v>
       </c>
-      <c r="C9" s="69" t="s">
-        <v>74</v>
+      <c r="C9" s="85" t="s">
+        <v>72</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <v>2</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>34</v>
@@ -2709,31 +2738,31 @@
       <c r="M9" s="2">
         <v>-30</v>
       </c>
-      <c r="N9" s="83">
+      <c r="N9" s="93">
         <v>-15</v>
       </c>
-      <c r="O9" s="84" t="s">
+      <c r="O9" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="P9" s="153" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q9" s="84"/>
+      <c r="P9" s="95" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q9" s="94"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="44">
+      <c r="B10" s="42">
         <v>4</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" s="23">
+        <v>74</v>
+      </c>
+      <c r="G10" s="22">
         <v>3</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>34</v>
@@ -2750,242 +2779,257 @@
       <c r="M10" s="8">
         <v>25</v>
       </c>
-      <c r="N10" s="77">
+      <c r="N10" s="81">
         <v>2</v>
       </c>
-      <c r="O10" s="78"/>
-      <c r="P10" s="77" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q10" s="78"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="81" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q10" s="82"/>
     </row>
     <row r="11" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="43">
+      <c r="B11" s="41">
         <v>5</v>
       </c>
-      <c r="C11" s="95" t="s">
-        <v>149</v>
+      <c r="C11" s="72" t="s">
+        <v>145</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="83"/>
+      <c r="O11" s="83"/>
+      <c r="P11" s="83"/>
+      <c r="Q11" s="83"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="44">
+      <c r="B12" s="42">
         <v>6</v>
       </c>
-      <c r="C12" s="96"/>
+      <c r="C12" s="73"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="49"/>
-      <c r="P12" s="79"/>
-      <c r="Q12" s="79"/>
+        <v>146</v>
+      </c>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="80"/>
+      <c r="Q12" s="80"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="61">
+      <c r="B13" s="59">
         <v>7</v>
       </c>
-      <c r="C13" s="97"/>
+      <c r="C13" s="74"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="60" t="s">
-        <v>151</v>
-      </c>
-      <c r="G13" s="48"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="79"/>
-      <c r="O13" s="79"/>
-      <c r="P13" s="79"/>
-      <c r="Q13" s="79"/>
+      <c r="E13" s="58" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" s="46"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="80"/>
+      <c r="P13" s="80"/>
+      <c r="Q13" s="80"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="43">
+      <c r="B14" s="41">
         <v>8</v>
       </c>
-      <c r="C14" s="93" t="s">
-        <v>77</v>
+      <c r="C14" s="70" t="s">
+        <v>75</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="82"/>
-      <c r="O14" s="82"/>
-      <c r="P14" s="80"/>
-      <c r="Q14" s="80"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="84"/>
+      <c r="O14" s="84"/>
+      <c r="P14" s="79"/>
+      <c r="Q14" s="79"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="44">
+      <c r="B15" s="42">
         <v>9</v>
       </c>
-      <c r="C15" s="94"/>
+      <c r="C15" s="71"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="48"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="78"/>
+      <c r="O15" s="78"/>
+      <c r="P15" s="79"/>
+      <c r="Q15" s="79"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="41">
+        <v>10</v>
+      </c>
+      <c r="C16" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="G15" s="50"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="92"/>
-      <c r="O15" s="92"/>
-      <c r="P15" s="80"/>
-      <c r="Q15" s="80"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="43">
-        <v>10</v>
-      </c>
-      <c r="C16" s="93" t="s">
-        <v>81</v>
-      </c>
       <c r="D16" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="92"/>
-      <c r="O16" s="92"/>
-      <c r="P16" s="80"/>
-      <c r="Q16" s="80"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="78"/>
+      <c r="O16" s="78"/>
+      <c r="P16" s="79"/>
+      <c r="Q16" s="79"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="44">
+      <c r="B17" s="42">
         <v>11</v>
       </c>
-      <c r="C17" s="94"/>
+      <c r="C17" s="71"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G17" s="50"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="92"/>
-      <c r="O17" s="92"/>
-      <c r="P17" s="80"/>
-      <c r="Q17" s="80"/>
+        <v>80</v>
+      </c>
+      <c r="G17" s="48"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="78"/>
+      <c r="O17" s="78"/>
+      <c r="P17" s="79"/>
+      <c r="Q17" s="79"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="43">
+      <c r="B18" s="41">
         <v>12</v>
       </c>
-      <c r="C18" s="93" t="s">
-        <v>78</v>
+      <c r="C18" s="70" t="s">
+        <v>76</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="92"/>
-      <c r="O18" s="92"/>
-      <c r="P18" s="80"/>
-      <c r="Q18" s="80"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="78"/>
+      <c r="O18" s="78"/>
+      <c r="P18" s="79"/>
+      <c r="Q18" s="79"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="44">
+      <c r="B19" s="42">
         <v>13</v>
       </c>
-      <c r="C19" s="94"/>
+      <c r="C19" s="71"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="17"/>
-      <c r="N19" s="92"/>
-      <c r="O19" s="92"/>
-      <c r="P19" s="80"/>
-      <c r="Q19" s="80"/>
+        <v>78</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="N19" s="78"/>
+      <c r="O19" s="78"/>
+      <c r="P19" s="79"/>
+      <c r="Q19" s="79"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="43">
+      <c r="B20" s="41">
         <v>14</v>
       </c>
-      <c r="C20" s="93" t="s">
-        <v>83</v>
+      <c r="C20" s="70" t="s">
+        <v>81</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="44">
+      <c r="B21" s="42">
         <v>15</v>
       </c>
-      <c r="C21" s="94"/>
+      <c r="C21" s="71"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="91"/>
-      <c r="G22" s="91"/>
+        <v>35</v>
+      </c>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="G5:Q5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="H6:H7"/>
     <mergeCell ref="P7:Q7"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="N15:O15"/>
@@ -3002,26 +3046,11 @@
     <mergeCell ref="P14:Q14"/>
     <mergeCell ref="N13:O13"/>
     <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="G5:Q5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="I6:O6"/>
-    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C11:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3034,8 +3063,8 @@
   </sheetPr>
   <dimension ref="B1:R46"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11:R11"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3059,706 +3088,710 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
     </row>
     <row r="3" spans="2:18" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="70" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="72"/>
+      <c r="B3" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="88"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="116" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="116"/>
-      <c r="D5" s="116"/>
+      <c r="B5" s="108" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
       <c r="E5" s="3"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="102" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="103"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="103"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="103"/>
-      <c r="N5" s="103"/>
-      <c r="O5" s="103"/>
-      <c r="P5" s="103"/>
-      <c r="Q5" s="103"/>
-      <c r="R5" s="104"/>
+      <c r="H5" s="112" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="113"/>
+      <c r="J5" s="113"/>
+      <c r="K5" s="113"/>
+      <c r="L5" s="113"/>
+      <c r="M5" s="113"/>
+      <c r="N5" s="113"/>
+      <c r="O5" s="113"/>
+      <c r="P5" s="113"/>
+      <c r="Q5" s="113"/>
+      <c r="R5" s="114"/>
     </row>
     <row r="6" spans="2:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="H6" s="75" t="s">
+      <c r="H6" s="91" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="113" t="s">
+      <c r="J6" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="105" t="s">
+      <c r="K6" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="110"/>
+      <c r="M6" s="110"/>
+      <c r="N6" s="110"/>
+      <c r="O6" s="110"/>
+      <c r="P6" s="111"/>
+      <c r="Q6" s="109" t="s">
+        <v>30</v>
+      </c>
+      <c r="R6" s="111"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="70">
+        <v>1</v>
+      </c>
+      <c r="C7" s="102" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="92"/>
+      <c r="I7" s="105"/>
+      <c r="J7" s="116"/>
+      <c r="K7" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q7" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="107" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="117"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="108"/>
-      <c r="Q6" s="107" t="s">
-        <v>30</v>
-      </c>
-      <c r="R6" s="108"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="93">
-        <v>1</v>
-      </c>
-      <c r="C7" s="98" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7" s="62" t="s">
-        <v>97</v>
-      </c>
-      <c r="H7" s="76"/>
-      <c r="I7" s="113"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="M7" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="N7" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="P7" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q7" s="85" t="s">
-        <v>43</v>
-      </c>
-      <c r="R7" s="86"/>
+      <c r="R7" s="76"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="101"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="62" t="s">
-        <v>98</v>
-      </c>
-      <c r="H8" s="13">
+      <c r="C8" s="103"/>
+      <c r="D8" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="12">
         <v>1</v>
       </c>
-      <c r="I8" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="J8" s="40" t="s">
-        <v>141</v>
-      </c>
-      <c r="K8" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="L8" s="21">
+      <c r="I8" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="20">
         <v>1</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="20">
         <v>2</v>
       </c>
-      <c r="N8" s="21">
+      <c r="N8" s="20">
         <v>1</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="20">
         <v>10</v>
       </c>
-      <c r="P8" s="21">
+      <c r="P8" s="20">
         <v>100</v>
       </c>
-      <c r="Q8" s="109" t="s">
-        <v>91</v>
-      </c>
-      <c r="R8" s="110"/>
-    </row>
-    <row r="9" spans="2:18" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q8" s="117" t="s">
+        <v>89</v>
+      </c>
+      <c r="R8" s="118"/>
+    </row>
+    <row r="9" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="101"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="63" t="s">
-        <v>99</v>
+      <c r="C9" s="103"/>
+      <c r="D9" s="61" t="s">
+        <v>97</v>
       </c>
       <c r="H9" s="10">
         <v>2</v>
       </c>
-      <c r="I9" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="J9" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="9">
-        <v>-1</v>
+      <c r="I9" s="155" t="s">
+        <v>157</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="L9" s="20">
+        <v>50</v>
       </c>
       <c r="M9" s="9">
-        <v>-15</v>
-      </c>
-      <c r="N9" s="9">
-        <v>-1</v>
-      </c>
-      <c r="O9" s="9">
-        <v>-15</v>
-      </c>
-      <c r="P9" s="9">
-        <v>-1</v>
-      </c>
-      <c r="Q9" s="154" t="s">
-        <v>154</v>
-      </c>
-      <c r="R9" s="111"/>
+        <v>1</v>
+      </c>
+      <c r="N9" s="20">
+        <v>2</v>
+      </c>
+      <c r="O9" s="20">
+        <v>3</v>
+      </c>
+      <c r="P9" s="20">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="119" t="s">
+        <v>158</v>
+      </c>
+      <c r="R9" s="120"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="101"/>
-      <c r="C10" s="99"/>
-      <c r="D10" s="63" t="s">
-        <v>100</v>
-      </c>
-      <c r="H10" s="13">
+      <c r="C10" s="103"/>
+      <c r="D10" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="H10" s="12">
         <v>3</v>
       </c>
-      <c r="I10" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="J10" s="40" t="s">
-        <v>141</v>
-      </c>
-      <c r="K10" s="20" t="s">
+      <c r="I10" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="20">
+        <v>2</v>
+      </c>
+      <c r="M10" s="20">
+        <v>50</v>
+      </c>
+      <c r="N10" s="20">
         <v>45</v>
       </c>
-      <c r="L10" s="21">
-        <v>2</v>
-      </c>
-      <c r="M10" s="21">
-        <v>50</v>
-      </c>
-      <c r="N10" s="21">
+      <c r="O10" s="20">
+        <v>99</v>
+      </c>
+      <c r="P10" s="20">
         <v>45</v>
       </c>
-      <c r="O10" s="21">
+      <c r="Q10" s="117" t="s">
+        <v>89</v>
+      </c>
+      <c r="R10" s="118"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="101"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="61" t="s">
         <v>99</v>
-      </c>
-      <c r="P10" s="21">
-        <v>45</v>
-      </c>
-      <c r="Q10" s="109" t="s">
-        <v>91</v>
-      </c>
-      <c r="R10" s="110"/>
-    </row>
-    <row r="11" spans="2:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="101"/>
-      <c r="C11" s="99"/>
-      <c r="D11" s="63" t="s">
-        <v>101</v>
       </c>
       <c r="H11" s="10">
         <v>4</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="K11" s="56" t="s">
-        <v>46</v>
+        <v>153</v>
+      </c>
+      <c r="J11" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="K11" s="54" t="s">
+        <v>44</v>
       </c>
       <c r="L11" s="2">
         <v>2</v>
       </c>
-      <c r="M11" s="2">
-        <v>1</v>
+      <c r="M11" s="9">
+        <v>101</v>
       </c>
       <c r="N11" s="2">
         <v>1</v>
       </c>
-      <c r="O11" s="9">
-        <v>-10</v>
-      </c>
-      <c r="P11" s="9">
+      <c r="O11" s="157">
+        <v>100</v>
+      </c>
+      <c r="P11" s="20">
         <v>1</v>
       </c>
-      <c r="Q11" s="154" t="s">
-        <v>156</v>
-      </c>
-      <c r="R11" s="111"/>
+      <c r="Q11" s="119" t="s">
+        <v>158</v>
+      </c>
+      <c r="R11" s="120"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="94"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="62" t="s">
+      <c r="B12" s="71"/>
+      <c r="C12" s="104"/>
+      <c r="D12" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="H12" s="16"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="53"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="53"/>
+      <c r="Q12" s="100"/>
+      <c r="R12" s="100"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="70">
+        <v>2</v>
+      </c>
+      <c r="C13" s="70" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="61" t="s">
         <v>102</v>
-      </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="55"/>
-      <c r="P12" s="55"/>
-      <c r="Q12" s="112"/>
-      <c r="R12" s="112"/>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="93">
-        <v>2</v>
-      </c>
-      <c r="C13" s="93" t="s">
-        <v>103</v>
-      </c>
-      <c r="D13" s="63" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="101"/>
       <c r="C14" s="101"/>
-      <c r="D14" s="63" t="s">
-        <v>111</v>
-      </c>
-      <c r="H14" s="17"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="55"/>
-      <c r="N14" s="55"/>
-      <c r="O14" s="55"/>
-      <c r="P14" s="55"/>
-      <c r="Q14" s="112"/>
-      <c r="R14" s="112"/>
+      <c r="D14" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="53"/>
+      <c r="O14" s="53"/>
+      <c r="P14" s="53"/>
+      <c r="Q14" s="100"/>
+      <c r="R14" s="100"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="101"/>
       <c r="C15" s="101"/>
-      <c r="D15" s="62" t="s">
-        <v>112</v>
-      </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="55"/>
-      <c r="M15" s="55"/>
-      <c r="N15" s="55"/>
-      <c r="O15" s="55"/>
-      <c r="P15" s="55"/>
-      <c r="Q15" s="112"/>
-      <c r="R15" s="112"/>
+      <c r="D15" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="53"/>
+      <c r="Q15" s="100"/>
+      <c r="R15" s="100"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="94"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="63" t="s">
-        <v>145</v>
-      </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="55"/>
-      <c r="M16" s="55"/>
-      <c r="N16" s="55"/>
-      <c r="O16" s="55"/>
-      <c r="P16" s="55"/>
-      <c r="Q16" s="112"/>
-      <c r="R16" s="112"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="61" t="s">
+        <v>141</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="53"/>
+      <c r="P16" s="53"/>
+      <c r="Q16" s="100"/>
+      <c r="R16" s="100"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="93">
+      <c r="B17" s="70">
         <v>3</v>
       </c>
-      <c r="C17" s="98" t="s">
-        <v>152</v>
-      </c>
-      <c r="D17" s="63" t="s">
-        <v>105</v>
-      </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="55"/>
-      <c r="M17" s="55"/>
-      <c r="N17" s="55"/>
-      <c r="O17" s="55"/>
-      <c r="P17" s="55"/>
-      <c r="Q17" s="112"/>
-      <c r="R17" s="112"/>
+      <c r="C17" s="102" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="61" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="100"/>
+      <c r="R17" s="100"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="101"/>
-      <c r="C18" s="99"/>
-      <c r="D18" s="63" t="s">
-        <v>106</v>
-      </c>
-      <c r="H18" s="17"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="55"/>
-      <c r="L18" s="55"/>
-      <c r="M18" s="55"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="55"/>
-      <c r="P18" s="55"/>
-      <c r="Q18" s="112"/>
-      <c r="R18" s="112"/>
+      <c r="C18" s="103"/>
+      <c r="D18" s="61" t="s">
+        <v>104</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="53"/>
+      <c r="O18" s="53"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="100"/>
+      <c r="R18" s="100"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="101"/>
-      <c r="C19" s="99"/>
-      <c r="D19" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="55"/>
-      <c r="L19" s="55"/>
-      <c r="M19" s="55"/>
-      <c r="N19" s="55"/>
-      <c r="O19" s="55"/>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="112"/>
-      <c r="R19" s="112"/>
+      <c r="C19" s="103"/>
+      <c r="D19" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="53"/>
+      <c r="O19" s="53"/>
+      <c r="P19" s="53"/>
+      <c r="Q19" s="100"/>
+      <c r="R19" s="100"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="101"/>
-      <c r="C20" s="99"/>
-      <c r="D20" s="62" t="s">
-        <v>108</v>
-      </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="55"/>
-      <c r="L20" s="55"/>
-      <c r="M20" s="55"/>
-      <c r="N20" s="55"/>
-      <c r="O20" s="55"/>
-      <c r="P20" s="55"/>
-      <c r="Q20" s="112"/>
-      <c r="R20" s="112"/>
+      <c r="C20" s="103"/>
+      <c r="D20" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="53"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="100"/>
+      <c r="R20" s="100"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="101"/>
-      <c r="C21" s="99"/>
-      <c r="D21" s="63" t="s">
-        <v>109</v>
-      </c>
-      <c r="H21" s="17"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="112"/>
-      <c r="R21" s="112"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="60" t="s">
+        <v>156</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
+      <c r="N21" s="53"/>
+      <c r="O21" s="53"/>
+      <c r="P21" s="53"/>
+      <c r="Q21" s="100"/>
+      <c r="R21" s="100"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="94"/>
-      <c r="C22" s="100"/>
-      <c r="D22" s="63" t="s">
+      <c r="B22" s="71"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="53"/>
+      <c r="P22" s="53"/>
+      <c r="Q22" s="100"/>
+      <c r="R22" s="100"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B23" s="70">
+        <v>4</v>
+      </c>
+      <c r="C23" s="102" t="s">
         <v>110</v>
       </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="55"/>
-      <c r="L22" s="55"/>
-      <c r="M22" s="55"/>
-      <c r="N22" s="55"/>
-      <c r="O22" s="55"/>
-      <c r="P22" s="55"/>
-      <c r="Q22" s="112"/>
-      <c r="R22" s="112"/>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="93">
-        <v>4</v>
-      </c>
-      <c r="C23" s="98" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" s="63" t="s">
-        <v>114</v>
-      </c>
-      <c r="H23" s="17"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="55"/>
-      <c r="M23" s="55"/>
-      <c r="N23" s="55"/>
-      <c r="O23" s="55"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="112"/>
-      <c r="R23" s="112"/>
+      <c r="D23" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="H23" s="16"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="53"/>
+      <c r="Q23" s="100"/>
+      <c r="R23" s="100"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="101"/>
-      <c r="C24" s="99"/>
-      <c r="D24" s="63" t="s">
-        <v>115</v>
-      </c>
-      <c r="H24" s="17"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="55"/>
-      <c r="L24" s="55"/>
-      <c r="M24" s="55"/>
-      <c r="N24" s="55"/>
-      <c r="O24" s="55"/>
-      <c r="P24" s="55"/>
-      <c r="Q24" s="112"/>
-      <c r="R24" s="112"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="53"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="53"/>
+      <c r="O24" s="53"/>
+      <c r="P24" s="53"/>
+      <c r="Q24" s="100"/>
+      <c r="R24" s="100"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="101"/>
-      <c r="C25" s="99"/>
-      <c r="D25" s="62" t="s">
-        <v>116</v>
-      </c>
-      <c r="H25" s="17"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="55"/>
-      <c r="L25" s="55"/>
-      <c r="M25" s="55"/>
-      <c r="N25" s="55"/>
-      <c r="O25" s="55"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="112"/>
-      <c r="R25" s="112"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="H25" s="16"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="53"/>
+      <c r="P25" s="53"/>
+      <c r="Q25" s="100"/>
+      <c r="R25" s="100"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="101"/>
-      <c r="C26" s="99"/>
-      <c r="D26" s="63" t="s">
-        <v>117</v>
+      <c r="C26" s="103"/>
+      <c r="D26" s="61" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="101"/>
-      <c r="C27" s="99"/>
-      <c r="D27" s="63" t="s">
+      <c r="C27" s="103"/>
+      <c r="D27" s="61" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="71"/>
+      <c r="C28" s="104"/>
+      <c r="D28" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="77"/>
+      <c r="H28" s="77"/>
+      <c r="I28" s="107"/>
+      <c r="J28" s="107"/>
+      <c r="K28" s="107"/>
+      <c r="L28" s="107"/>
+      <c r="M28" s="107"/>
+      <c r="N28" s="29"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="70">
+        <v>5</v>
+      </c>
+      <c r="C29" s="102" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="61" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="94"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="62" t="s">
-        <v>119</v>
-      </c>
-      <c r="G28" s="91"/>
-      <c r="H28" s="91"/>
-      <c r="I28" s="115"/>
-      <c r="J28" s="115"/>
-      <c r="K28" s="115"/>
-      <c r="L28" s="115"/>
-      <c r="M28" s="115"/>
-      <c r="N28" s="30"/>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="93">
-        <v>5</v>
-      </c>
-      <c r="C29" s="98" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29" s="63" t="s">
-        <v>121</v>
-      </c>
-      <c r="I29" s="114"/>
-      <c r="J29" s="114"/>
-      <c r="K29" s="114"/>
-      <c r="L29" s="114"/>
-      <c r="M29" s="114"/>
-      <c r="N29" s="31"/>
+      <c r="I29" s="106"/>
+      <c r="J29" s="106"/>
+      <c r="K29" s="106"/>
+      <c r="L29" s="106"/>
+      <c r="M29" s="106"/>
+      <c r="N29" s="30"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="101"/>
-      <c r="C30" s="99"/>
-      <c r="D30" s="63" t="s">
-        <v>122</v>
+      <c r="C30" s="103"/>
+      <c r="D30" s="61" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="101"/>
-      <c r="C31" s="99"/>
-      <c r="D31" s="62" t="s">
-        <v>123</v>
+      <c r="C31" s="103"/>
+      <c r="D31" s="60" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="101"/>
-      <c r="C32" s="99"/>
-      <c r="D32" s="62" t="s">
-        <v>124</v>
+      <c r="C32" s="103"/>
+      <c r="D32" s="60" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="101"/>
-      <c r="C33" s="99"/>
-      <c r="D33" s="62" t="s">
+      <c r="C33" s="103"/>
+      <c r="D33" s="60" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="71"/>
+      <c r="C34" s="104"/>
+      <c r="D34" s="60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="70">
+        <v>6</v>
+      </c>
+      <c r="C35" s="102" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="61" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="94"/>
-      <c r="C34" s="100"/>
-      <c r="D34" s="62" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="93">
-        <v>6</v>
-      </c>
-      <c r="C35" s="98" t="s">
-        <v>127</v>
-      </c>
-      <c r="D35" s="63" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="101"/>
-      <c r="C36" s="99"/>
-      <c r="D36" s="63" t="s">
-        <v>129</v>
+      <c r="C36" s="103"/>
+      <c r="D36" s="61" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="101"/>
-      <c r="C37" s="99"/>
-      <c r="D37" s="63" t="s">
-        <v>130</v>
+      <c r="C37" s="103"/>
+      <c r="D37" s="61" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="101"/>
-      <c r="C38" s="99"/>
-      <c r="D38" s="63" t="s">
-        <v>131</v>
+      <c r="C38" s="103"/>
+      <c r="D38" s="61" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="101"/>
-      <c r="C39" s="99"/>
-      <c r="D39" s="62" t="s">
+      <c r="C39" s="103"/>
+      <c r="D39" s="60" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="71"/>
+      <c r="C40" s="104"/>
+      <c r="D40" s="61" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="70">
+        <v>7</v>
+      </c>
+      <c r="C41" s="102" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" s="61" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="94"/>
-      <c r="C40" s="100"/>
-      <c r="D40" s="63" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="93">
-        <v>7</v>
-      </c>
-      <c r="C41" s="98" t="s">
-        <v>134</v>
-      </c>
-      <c r="D41" s="63" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="101"/>
-      <c r="C42" s="99"/>
-      <c r="D42" s="63" t="s">
-        <v>136</v>
+      <c r="C42" s="103"/>
+      <c r="D42" s="61" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="101"/>
-      <c r="C43" s="99"/>
-      <c r="D43" s="62" t="s">
-        <v>137</v>
+      <c r="C43" s="103"/>
+      <c r="D43" s="60" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="101"/>
-      <c r="C44" s="99"/>
-      <c r="D44" s="63" t="s">
-        <v>138</v>
+      <c r="C44" s="103"/>
+      <c r="D44" s="61" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="101"/>
-      <c r="C45" s="99"/>
-      <c r="D45" s="63" t="s">
-        <v>139</v>
+      <c r="C45" s="103"/>
+      <c r="D45" s="61" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="94"/>
-      <c r="C46" s="100"/>
-      <c r="D46" s="62" t="s">
-        <v>140</v>
+      <c r="B46" s="71"/>
+      <c r="C46" s="104"/>
+      <c r="D46" s="60" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="B35:B40"/>
+    <mergeCell ref="C35:C40"/>
+    <mergeCell ref="H5:R5"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="Q12:R12"/>
     <mergeCell ref="B41:B46"/>
     <mergeCell ref="C41:C46"/>
     <mergeCell ref="B1:E1"/>
@@ -3775,22 +3808,18 @@
     <mergeCell ref="B23:B28"/>
     <mergeCell ref="C23:C28"/>
     <mergeCell ref="B29:B34"/>
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="C35:C40"/>
-    <mergeCell ref="H5:R5"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="B17:B22"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="Q21:R21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3805,8 +3834,8 @@
   </sheetPr>
   <dimension ref="B1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10:L10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3821,103 +3850,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="128" t="s">
+      <c r="B3" s="154" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="154"/>
+      <c r="D3" s="154"/>
+      <c r="E3" s="154"/>
+      <c r="F3" s="154"/>
+      <c r="G3" s="154"/>
+      <c r="H3" s="154"/>
+      <c r="I3" s="154"/>
+      <c r="J3" s="154"/>
+      <c r="K3" s="154"/>
+      <c r="L3" s="154"/>
+      <c r="M3" s="154"/>
+      <c r="N3" s="154"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="91" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="148" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
-      <c r="N3" s="128"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="75" t="s">
+      <c r="D4" s="115" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="125" t="s">
+      <c r="E4" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="105" t="s">
+      <c r="F4" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="98" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="98"/>
+    </row>
+    <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="128"/>
+      <c r="C5" s="149"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="147"/>
+      <c r="F5" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="143" t="s">
+        <v>88</v>
+      </c>
+      <c r="L5" s="144"/>
+      <c r="M5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="87" t="s">
+    </row>
+    <row r="6" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="13">
+        <v>1</v>
+      </c>
+      <c r="C6" s="134" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="85" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="89" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="89"/>
-    </row>
-    <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="129"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="124"/>
-      <c r="F5" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="K5" s="119" t="s">
-        <v>90</v>
-      </c>
-      <c r="L5" s="120"/>
-      <c r="M5" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" s="15" t="s">
+      <c r="D6" s="17" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="14">
-        <v>1</v>
-      </c>
-      <c r="C6" s="136" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G6" s="2">
         <v>100</v>
@@ -3931,17 +3960,17 @@
       <c r="J6" s="2">
         <v>30</v>
       </c>
-      <c r="K6" s="121">
+      <c r="K6" s="145">
         <v>5</v>
       </c>
-      <c r="L6" s="122" t="s">
+      <c r="L6" s="146" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="57" t="s">
-        <v>91</v>
-      </c>
-      <c r="N6" s="57" t="s">
-        <v>91</v>
+      <c r="M6" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="N6" s="55" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="105" x14ac:dyDescent="0.25">
@@ -3949,9 +3978,9 @@
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="137"/>
-      <c r="D7" s="19" t="s">
-        <v>148</v>
+      <c r="C7" s="135"/>
+      <c r="D7" s="18" t="s">
+        <v>144</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>33</v>
@@ -3971,17 +4000,17 @@
       <c r="J7" s="9">
         <v>-30</v>
       </c>
-      <c r="K7" s="156">
+      <c r="K7" s="150">
         <v>-15</v>
       </c>
-      <c r="L7" s="157" t="s">
+      <c r="L7" s="151" t="s">
         <v>33</v>
       </c>
-      <c r="M7" s="150" t="s">
-        <v>154</v>
-      </c>
-      <c r="N7" s="150" t="s">
-        <v>154</v>
+      <c r="M7" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="N7" s="62" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
@@ -3989,9 +4018,9 @@
         <f t="shared" ref="B8:B12" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="137"/>
-      <c r="D8" s="19" t="s">
-        <v>55</v>
+      <c r="C8" s="135"/>
+      <c r="D8" s="18" t="s">
+        <v>53</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>33</v>
@@ -4011,15 +4040,15 @@
       <c r="J8" s="2">
         <v>25</v>
       </c>
-      <c r="K8" s="83">
+      <c r="K8" s="93">
         <v>2</v>
       </c>
-      <c r="L8" s="84"/>
+      <c r="L8" s="94"/>
       <c r="M8" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
@@ -4027,75 +4056,75 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="137"/>
-      <c r="D9" s="19" t="s">
+      <c r="C9" s="135"/>
+      <c r="D9" s="18" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="21">
+        <v>142</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="20">
         <v>1</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="20">
         <v>0</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="20">
         <v>1</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="20">
         <v>10</v>
       </c>
-      <c r="K9" s="127">
+      <c r="K9" s="152">
         <v>100</v>
       </c>
-      <c r="L9" s="127"/>
-      <c r="M9" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="N9" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="L9" s="152"/>
+      <c r="M9" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="N9" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="137"/>
-      <c r="D10" s="19" t="s">
+      <c r="C10" s="135"/>
+      <c r="D10" s="18" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="9">
-        <v>-1</v>
+        <v>143</v>
+      </c>
+      <c r="F10" s="156" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" s="157">
+        <v>50</v>
       </c>
       <c r="H10" s="9">
-        <v>-15</v>
-      </c>
-      <c r="I10" s="9">
-        <v>-1</v>
-      </c>
-      <c r="J10" s="9">
-        <v>-15</v>
-      </c>
-      <c r="K10" s="123">
-        <v>-1</v>
-      </c>
-      <c r="L10" s="123"/>
-      <c r="M10" s="151" t="s">
-        <v>154</v>
-      </c>
-      <c r="N10" s="152" t="s">
-        <v>154</v>
+        <v>1</v>
+      </c>
+      <c r="I10" s="157">
+        <v>2</v>
+      </c>
+      <c r="J10" s="157">
+        <v>3</v>
+      </c>
+      <c r="K10" s="158">
+        <v>2</v>
+      </c>
+      <c r="L10" s="158"/>
+      <c r="M10" s="63" t="s">
+        <v>158</v>
+      </c>
+      <c r="N10" s="64" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
@@ -4103,37 +4132,37 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="137"/>
-      <c r="D11" s="19" t="s">
+      <c r="C11" s="135"/>
+      <c r="D11" s="18" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="20">
+        <v>2</v>
+      </c>
+      <c r="H11" s="20">
+        <v>100</v>
+      </c>
+      <c r="I11" s="20">
         <v>45</v>
       </c>
-      <c r="G11" s="21">
-        <v>2</v>
-      </c>
-      <c r="H11" s="21">
-        <v>100</v>
-      </c>
-      <c r="I11" s="21">
+      <c r="J11" s="20">
+        <v>99</v>
+      </c>
+      <c r="K11" s="152">
         <v>45</v>
       </c>
-      <c r="J11" s="21">
-        <v>99</v>
-      </c>
-      <c r="K11" s="127">
-        <v>45</v>
-      </c>
-      <c r="L11" s="127"/>
-      <c r="M11" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="N11" s="21" t="s">
-        <v>91</v>
+      <c r="L11" s="152"/>
+      <c r="M11" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="N11" s="20" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="45" x14ac:dyDescent="0.25">
@@ -4141,212 +4170,212 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="138"/>
-      <c r="D12" s="19" t="s">
+      <c r="C12" s="136"/>
+      <c r="D12" s="18" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="56" t="s">
-        <v>46</v>
+        <v>55</v>
+      </c>
+      <c r="F12" s="54" t="s">
+        <v>44</v>
       </c>
       <c r="G12" s="2">
         <v>2</v>
       </c>
-      <c r="H12" s="2">
-        <v>1</v>
+      <c r="H12" s="9">
+        <v>101</v>
       </c>
       <c r="I12" s="2">
         <v>1</v>
       </c>
-      <c r="J12" s="9">
-        <v>-10</v>
-      </c>
-      <c r="K12" s="155">
+      <c r="J12" s="157">
+        <v>100</v>
+      </c>
+      <c r="K12" s="153">
         <v>0</v>
       </c>
-      <c r="L12" s="155"/>
-      <c r="M12" s="151" t="s">
-        <v>156</v>
-      </c>
-      <c r="N12" s="152" t="s">
-        <v>156</v>
+      <c r="L12" s="153"/>
+      <c r="M12" s="63" t="s">
+        <v>152</v>
+      </c>
+      <c r="N12" s="64" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="16"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="118"/>
-      <c r="L13" s="118"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="142"/>
+      <c r="L13" s="142"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
     </row>
     <row r="15" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="16"/>
+      <c r="B15" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="15"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="92"/>
-      <c r="L15" s="92"/>
+      <c r="K15" s="78"/>
+      <c r="L15" s="78"/>
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="139" t="s">
+      <c r="C17" s="122" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="124"/>
+      <c r="E17" s="124"/>
+      <c r="F17" s="125"/>
+      <c r="G17" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="122" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="140"/>
-      <c r="E17" s="140"/>
-      <c r="F17" s="141"/>
-      <c r="G17" s="26" t="s">
+      <c r="I17" s="123"/>
+      <c r="J17" s="124"/>
+      <c r="K17" s="124"/>
+      <c r="L17" s="125"/>
+      <c r="M17" s="122" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="139" t="s">
+      <c r="N17" s="123"/>
+      <c r="O17" s="124"/>
+      <c r="P17" s="125"/>
+    </row>
+    <row r="18" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="132" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="133" t="s">
         <v>61</v>
       </c>
-      <c r="I17" s="142"/>
-      <c r="J17" s="140"/>
-      <c r="K17" s="140"/>
-      <c r="L17" s="141"/>
-      <c r="M17" s="139" t="s">
+      <c r="D18" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="N17" s="142"/>
-      <c r="O17" s="140"/>
-      <c r="P17" s="141"/>
-    </row>
-    <row r="18" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="133" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="134" t="s">
+      <c r="E18" s="105" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="113" t="s">
+      <c r="F18" s="121" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="113" t="s">
+      <c r="G18" s="141" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="135" t="s">
+      <c r="H18" s="137" t="s">
         <v>66</v>
       </c>
-      <c r="G18" s="147" t="s">
+      <c r="I18" s="138"/>
+      <c r="J18" s="105" t="s">
+        <v>61</v>
+      </c>
+      <c r="K18" s="105" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" s="121" t="s">
+        <v>63</v>
+      </c>
+      <c r="M18" s="126" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" s="105" t="s">
+        <v>61</v>
+      </c>
+      <c r="O18" s="105" t="s">
+        <v>62</v>
+      </c>
+      <c r="P18" s="121" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="132"/>
+      <c r="C19" s="133"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="105"/>
+      <c r="F19" s="121"/>
+      <c r="G19" s="141"/>
+      <c r="H19" s="139"/>
+      <c r="I19" s="140"/>
+      <c r="J19" s="105"/>
+      <c r="K19" s="105"/>
+      <c r="L19" s="121"/>
+      <c r="M19" s="127"/>
+      <c r="N19" s="105"/>
+      <c r="O19" s="105"/>
+      <c r="P19" s="121"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="24">
+        <v>7</v>
+      </c>
+      <c r="D20" s="26">
+        <v>7</v>
+      </c>
+      <c r="E20" s="26">
+        <v>0</v>
+      </c>
+      <c r="F20" s="27"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="130" t="s">
         <v>67</v>
       </c>
-      <c r="H18" s="143" t="s">
-        <v>68</v>
-      </c>
-      <c r="I18" s="144"/>
-      <c r="J18" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="K18" s="113" t="s">
-        <v>64</v>
-      </c>
-      <c r="L18" s="135" t="s">
-        <v>65</v>
-      </c>
-      <c r="M18" s="148" t="s">
-        <v>68</v>
-      </c>
-      <c r="N18" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="O18" s="113" t="s">
-        <v>64</v>
-      </c>
-      <c r="P18" s="135" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="133"/>
-      <c r="C19" s="134"/>
-      <c r="D19" s="113"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="135"/>
-      <c r="G19" s="147"/>
-      <c r="H19" s="145"/>
-      <c r="I19" s="146"/>
-      <c r="J19" s="113"/>
-      <c r="K19" s="113"/>
-      <c r="L19" s="135"/>
-      <c r="M19" s="149"/>
-      <c r="N19" s="113"/>
-      <c r="O19" s="113"/>
-      <c r="P19" s="135"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="25">
-        <v>7</v>
-      </c>
-      <c r="D20" s="27">
-        <v>7</v>
-      </c>
-      <c r="E20" s="27">
-        <v>0</v>
-      </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="131" t="s">
-        <v>69</v>
-      </c>
-      <c r="I20" s="132"/>
+      <c r="I20" s="131"/>
       <c r="J20" s="2">
         <v>3</v>
       </c>
-      <c r="K20" s="27">
+      <c r="K20" s="26">
         <v>3</v>
       </c>
-      <c r="L20" s="28">
+      <c r="L20" s="27">
         <v>0</v>
       </c>
-      <c r="M20" s="32" t="s">
-        <v>69</v>
+      <c r="M20" s="31" t="s">
+        <v>67</v>
       </c>
       <c r="N20" s="2">
         <v>5</v>
       </c>
-      <c r="O20" s="27">
+      <c r="O20" s="26">
         <v>5</v>
       </c>
-      <c r="P20" s="28">
+      <c r="P20" s="27">
         <v>0</v>
       </c>
     </row>
@@ -4355,13 +4384,20 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F4:L4"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="B3:N3"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
@@ -4378,20 +4414,13 @@
     <mergeCell ref="H17:L17"/>
     <mergeCell ref="H18:I19"/>
     <mergeCell ref="G18:G19"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F4:L4"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4400,21 +4429,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5F472198D7887469049920058585067" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e76e8f6ca957e849a493f1baa4f4bb7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c46c0853-0d59-45c6-b517-3e25eac8cdf1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ddeb00cc2097713d6f56fe4f26be38f" ns2:_="">
     <xsd:import namespace="c46c0853-0d59-45c6-b517-3e25eac8cdf1"/>
@@ -4558,24 +4572,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B0A340A-7B8D-463A-B976-63A023B5D9BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153A5999-B236-48B1-944C-C5EB94545735}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4591,4 +4603,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B0A340A-7B8D-463A-B976-63A023B5D9BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>